<commit_message>
989: changes to make new team in ND02 file
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND02.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND02.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="103">
   <si>
     <t>Trust</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Farringdon</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>KainosLDU</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t>ND01</t>
   </si>
   <si>
     <t>LicenceTier0</t>
@@ -341,6 +335,21 @@
   </si>
   <si>
     <t>Andy Wright</t>
+  </si>
+  <si>
+    <t>ND02</t>
+  </si>
+  <si>
+    <t>Swann II</t>
+  </si>
+  <si>
+    <t>Wright II</t>
+  </si>
+  <si>
+    <t>WMT (ND02)</t>
+  </si>
+  <si>
+    <t>London II</t>
   </si>
 </sst>
 </file>
@@ -778,7 +787,7 @@
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,28 +890,28 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>22</v>
@@ -943,31 +952,31 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
       </c>
       <c r="K2">
         <v>1004</v>
@@ -1068,31 +1077,31 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>43</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
       </c>
       <c r="K3">
         <v>1005</v>
@@ -1198,53 +1207,53 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>90</v>
-      </c>
-      <c r="M1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1255,40 +1264,40 @@
         <v>42991</v>
       </c>
       <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2">
+        <v>1004</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2">
-        <v>1001</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>96</v>
-      </c>
       <c r="K2">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1299,40 +1308,40 @@
         <v>42991</v>
       </c>
       <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
         <v>97</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3">
+        <v>1005</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
         <v>98</v>
       </c>
-      <c r="E3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3">
-        <v>1002</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K3">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1365,22 +1374,22 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>32</v>
@@ -1388,19 +1397,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="D2">
         <v>1004</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -1417,19 +1426,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>1005</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3">
         <v>18</v>
@@ -1477,19 +1486,19 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -1497,19 +1506,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="D2">
         <v>1004</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1523,19 +1532,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>1005</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1573,13 +1582,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1591,53 +1600,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1657,13 +1666,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1675,53 +1684,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1741,13 +1750,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1759,53 +1768,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1825,13 +1834,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1843,53 +1852,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>